<commit_message>
modificartions to calculate variance
</commit_message>
<xml_diff>
--- a/backend/auxiliar/LIGHT_2025-02-26_20-09-08_R_1x1_-10.00_3.00s_0011.astropy-units.xlsx
+++ b/backend/auxiliar/LIGHT_2025-02-26_20-09-08_R_1x1_-10.00_3.00s_0011.astropy-units.xlsx
@@ -716,16 +716,16 @@
         <v>0.4353475333248427</v>
       </c>
       <c r="AF2" t="n">
-        <v>0.1324733551977317</v>
+        <v>0.0001180168397070247</v>
       </c>
       <c r="AG2" t="n">
-        <v>1.265428775780141</v>
+        <v>7.043030873177258e-06</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.002312096219364362</v>
+        <v>2.059782425685961e-06</v>
       </c>
       <c r="AI2" t="n">
-        <v>0.02208589858684453</v>
+        <v>1.229240780565543e-07</v>
       </c>
     </row>
     <row r="3">
@@ -839,16 +839,16 @@
         <v>0.42430019487881</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.3116918826966923</v>
+        <v>-9.763669208950887e-05</v>
       </c>
       <c r="AG3" t="n">
-        <v>1.264956858384789</v>
+        <v>2.042721613548792e-05</v>
       </c>
       <c r="AH3" t="n">
-        <v>0.005440049604797223</v>
+        <v>-1.704081747717832e-06</v>
       </c>
       <c r="AI3" t="n">
-        <v>0.0220776620744982</v>
+        <v>3.565221785807764e-07</v>
       </c>
     </row>
     <row r="4">
@@ -962,16 +962,16 @@
         <v>0.4446012663728566</v>
       </c>
       <c r="AF4" t="n">
-        <v>-2.29879899555948</v>
+        <v>0.0005529119226252988</v>
       </c>
       <c r="AG4" t="n">
-        <v>1.240795236417913</v>
+        <v>0.0001569640776146741</v>
       </c>
       <c r="AH4" t="n">
-        <v>-0.04012161131405143</v>
+        <v>9.650133523343592e-06</v>
       </c>
       <c r="AI4" t="n">
-        <v>0.02165596221855403</v>
+        <v>2.73953996173199e-06</v>
       </c>
     </row>
     <row r="5">
@@ -1085,16 +1085,16 @@
         <v>0.4384854837564174</v>
       </c>
       <c r="AF5" t="n">
-        <v>-2.892605097527877</v>
+        <v>-0.0002319378970128128</v>
       </c>
       <c r="AG5" t="n">
-        <v>1.2335429021322</v>
+        <v>-1.761794495180879e-05</v>
       </c>
       <c r="AH5" t="n">
-        <v>-0.05048548291183314</v>
+        <v>-4.048079963025103e-06</v>
       </c>
       <c r="AI5" t="n">
-        <v>0.02152938510681307</v>
+        <v>-3.074911468441772e-07</v>
       </c>
     </row>
     <row r="6">
@@ -1208,16 +1208,16 @@
         <v>0.429922930702637</v>
       </c>
       <c r="AF6" t="n">
-        <v>-2.78906598241042</v>
+        <v>0.0001555432800444123</v>
       </c>
       <c r="AG6" t="n">
-        <v>1.233468318156358</v>
+        <v>1.860249967577943e-05</v>
       </c>
       <c r="AH6" t="n">
-        <v>-0.04867838444843209</v>
+        <v>2.714742366126587e-06</v>
       </c>
       <c r="AI6" t="n">
-        <v>0.0215280833708654</v>
+        <v>3.246748684435286e-07</v>
       </c>
     </row>
     <row r="7">
@@ -1331,16 +1331,16 @@
         <v>0.4137060486624825</v>
       </c>
       <c r="AF7" t="n">
-        <v>-1.08641179024292</v>
+        <v>1.406725147035104e-06</v>
       </c>
       <c r="AG7" t="n">
-        <v>1.247482303734895</v>
+        <v>-6.499588135255863e-06</v>
       </c>
       <c r="AH7" t="n">
-        <v>-0.01896146277222496</v>
+        <v>2.455198548636391e-08</v>
       </c>
       <c r="AI7" t="n">
-        <v>0.02177267356053787</v>
+        <v>-1.134392129837733e-07</v>
       </c>
     </row>
     <row r="8">
@@ -1454,16 +1454,16 @@
         <v>0.4483335937799197</v>
       </c>
       <c r="AF8" t="n">
-        <v>0.4171178931462975</v>
+        <v>4.557408715299971e-05</v>
       </c>
       <c r="AG8" t="n">
-        <v>1.269263718303982</v>
+        <v>1.121169369966424e-05</v>
       </c>
       <c r="AH8" t="n">
-        <v>0.007280080604384781</v>
+        <v>7.954178744106936e-07</v>
       </c>
       <c r="AI8" t="n">
-        <v>0.0221528309605103</v>
+        <v>1.956809697842452e-07</v>
       </c>
     </row>
     <row r="9">
@@ -1577,16 +1577,16 @@
         <v>0.4133090981006051</v>
       </c>
       <c r="AF9" t="n">
-        <v>0.5838312200132521</v>
+        <v>6.506150984364467e-05</v>
       </c>
       <c r="AG9" t="n">
-        <v>1.263816972546241</v>
+        <v>7.226120040115802e-07</v>
       </c>
       <c r="AH9" t="n">
-        <v>0.01018977706516666</v>
+        <v>1.135537563090301e-06</v>
       </c>
       <c r="AI9" t="n">
-        <v>0.02205776731351869</v>
+        <v>1.261195868443655e-08</v>
       </c>
     </row>
     <row r="10">
@@ -1700,16 +1700,16 @@
         <v>0.4338857468502161</v>
       </c>
       <c r="AF10" t="n">
-        <v>0.5066956287514586</v>
+        <v>-8.563498568037176e-05</v>
       </c>
       <c r="AG10" t="n">
-        <v>1.269038318056957</v>
+        <v>-6.624645177311095e-06</v>
       </c>
       <c r="AH10" t="n">
-        <v>0.008843507027175797</v>
+        <v>-1.494612455020684e-06</v>
       </c>
       <c r="AI10" t="n">
-        <v>0.02214889698406491</v>
+        <v>-1.156218701204422e-07</v>
       </c>
     </row>
     <row r="11">
@@ -1823,16 +1823,16 @@
         <v>0.4289595888309933</v>
       </c>
       <c r="AF11" t="n">
-        <v>-0.3765174570530121</v>
+        <v>9.742706333781825e-05</v>
       </c>
       <c r="AG11" t="n">
-        <v>1.259019150926107</v>
+        <v>2.122749405941704e-05</v>
       </c>
       <c r="AH11" t="n">
-        <v>-0.006571469316811407</v>
+        <v>1.700423035793985e-06</v>
       </c>
       <c r="AI11" t="n">
-        <v>0.02197402952932399</v>
+        <v>3.704896632843641e-07</v>
       </c>
     </row>
     <row r="12">
@@ -1946,16 +1946,16 @@
         <v>0.4507307116338873</v>
       </c>
       <c r="AF12" t="n">
-        <v>-1.340477458925392</v>
+        <v>-0.0001139440585689044</v>
       </c>
       <c r="AG12" t="n">
-        <v>1.251068299405613</v>
+        <v>-6.762308426644381e-05</v>
       </c>
       <c r="AH12" t="n">
-        <v>-0.02339574520701514</v>
+        <v>-1.98869898511264e-06</v>
       </c>
       <c r="AI12" t="n">
-        <v>0.02183526099195417</v>
+        <v>-1.180245470803019e-06</v>
       </c>
     </row>
     <row r="13">
@@ -2069,16 +2069,16 @@
         <v>0.4129163935052648</v>
       </c>
       <c r="AF13" t="n">
-        <v>-0.6749731410118613</v>
+        <v>-6.190919964410568e-05</v>
       </c>
       <c r="AG13" t="n">
-        <v>1.251330991176285</v>
+        <v>-1.899857210219125e-06</v>
       </c>
       <c r="AH13" t="n">
-        <v>-0.01178050367318495</v>
+        <v>-1.080519371064146e-06</v>
       </c>
       <c r="AI13" t="n">
-        <v>0.02183984582827029</v>
+        <v>-3.315876363607778e-08</v>
       </c>
     </row>
     <row r="14">
@@ -2192,16 +2192,16 @@
         <v>0.4367598123821324</v>
       </c>
       <c r="AF14" t="n">
-        <v>-2.621905058782261</v>
+        <v>-5.394209580344977e-05</v>
       </c>
       <c r="AG14" t="n">
-        <v>1.236321971782623</v>
+        <v>2.020891774634492e-05</v>
       </c>
       <c r="AH14" t="n">
-        <v>-0.04576087595044592</v>
+        <v>-9.414671771964145e-07</v>
       </c>
       <c r="AI14" t="n">
-        <v>0.02157788902235519</v>
+        <v>3.527121529384311e-07</v>
       </c>
     </row>
     <row r="15">
@@ -2315,16 +2315,16 @@
         <v>0.4461470514052666</v>
       </c>
       <c r="AF15" t="n">
-        <v>-1.541580986538492</v>
+        <v>-9.637072705004357e-05</v>
       </c>
       <c r="AG15" t="n">
-        <v>1.248951527319569</v>
+        <v>9.357044092439537e-05</v>
       </c>
       <c r="AH15" t="n">
-        <v>-0.02690566390123906</v>
+        <v>-1.681986489564022e-06</v>
       </c>
       <c r="AI15" t="n">
-        <v>0.02179831634953839</v>
+        <v>1.633112276673546e-06</v>
       </c>
     </row>
     <row r="16">
@@ -2438,16 +2438,16 @@
         <v>0.4322863023503487</v>
       </c>
       <c r="AF16" t="n">
-        <v>0.03066190126565971</v>
+        <v>8.870599910437704e-05</v>
       </c>
       <c r="AG16" t="n">
-        <v>1.263863285019021</v>
+        <v>-7.537564876258784e-06</v>
       </c>
       <c r="AH16" t="n">
-        <v>0.0005351511320071784</v>
+        <v>1.548211750642521e-06</v>
       </c>
       <c r="AI16" t="n">
-        <v>0.02205857561865343</v>
+        <v>-1.315553246733947e-07</v>
       </c>
     </row>
     <row r="17">
@@ -2561,16 +2561,16 @@
         <v>0.442182765359482</v>
       </c>
       <c r="AF17" t="n">
-        <v>-2.270503892927621</v>
+        <v>-0.0002119636181134865</v>
       </c>
       <c r="AG17" t="n">
-        <v>1.240530518520035</v>
+        <v>-0.0002107375396747102</v>
       </c>
       <c r="AH17" t="n">
-        <v>-0.03962776861093579</v>
+        <v>-3.699463030520231e-06</v>
       </c>
       <c r="AI17" t="n">
-        <v>0.02165134201964711</v>
+        <v>-3.678063924875873e-06</v>
       </c>
     </row>
     <row r="18">
@@ -2684,16 +2684,16 @@
         <v>0.4311444760383638</v>
       </c>
       <c r="AF18" t="n">
-        <v>0.4327723549161249</v>
+        <v>-8.169830471160822e-05</v>
       </c>
       <c r="AG18" t="n">
-        <v>1.267761275502988</v>
+        <v>-3.105098020128594e-05</v>
       </c>
       <c r="AH18" t="n">
-        <v>0.007553302504895847</v>
+        <v>-1.42590441051516e-06</v>
       </c>
       <c r="AI18" t="n">
-        <v>0.02212660838681007</v>
+        <v>-5.419418404840111e-07</v>
       </c>
     </row>
     <row r="19">
@@ -2807,16 +2807,16 @@
         <v>0.4388462108702269</v>
       </c>
       <c r="AF19" t="n">
-        <v>-1.500302958452096</v>
+        <v>-0.0001192559604135113</v>
       </c>
       <c r="AG19" t="n">
-        <v>1.248697829807085</v>
+        <v>1.236068153787073e-05</v>
       </c>
       <c r="AH19" t="n">
-        <v>-0.02618522640240076</v>
+        <v>-2.08140916184379e-06</v>
       </c>
       <c r="AI19" t="n">
-        <v>0.02179388849264143</v>
+        <v>2.157345906263204e-07</v>
       </c>
     </row>
     <row r="20">
@@ -2930,16 +2930,16 @@
         <v>0.4366516891924458</v>
       </c>
       <c r="AF20" t="n">
-        <v>0.3109276663373919</v>
+        <v>-5.736948804724307e-05</v>
       </c>
       <c r="AG20" t="n">
-        <v>1.267462540639499</v>
+        <v>1.80555296438456e-05</v>
       </c>
       <c r="AH20" t="n">
-        <v>0.005426711513129827</v>
+        <v>-1.001286456607924e-06</v>
       </c>
       <c r="AI20" t="n">
-        <v>0.0221213944798517</v>
+        <v>3.151284404765449e-07</v>
       </c>
     </row>
     <row r="21">
@@ -3053,16 +3053,16 @@
         <v>0.4364801799045143</v>
       </c>
       <c r="AF21" t="n">
-        <v>-0.2336545758333557</v>
+        <v>8.701560065560443e-05</v>
       </c>
       <c r="AG21" t="n">
-        <v>1.261748876141734</v>
+        <v>-3.080298937518933e-05</v>
       </c>
       <c r="AH21" t="n">
-        <v>-0.004078041660642831</v>
+        <v>1.518708732040834e-06</v>
       </c>
       <c r="AI21" t="n">
-        <v>0.02202167222201139</v>
+        <v>-5.376135840538846e-07</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
origen en centro foto
</commit_message>
<xml_diff>
--- a/backend/auxiliar/LIGHT_2025-02-26_20-09-08_R_1x1_-10.00_3.00s_0011.astropy-units.xlsx
+++ b/backend/auxiliar/LIGHT_2025-02-26_20-09-08_R_1x1_-10.00_3.00s_0011.astropy-units.xlsx
@@ -639,10 +639,10 @@
         <v>0.0001646357832762952</v>
       </c>
       <c r="K2" t="n">
-        <v>2071.004638671875</v>
+        <v>-256.995361328125</v>
       </c>
       <c r="L2" t="n">
-        <v>756.3301391601562</v>
+        <v>1003.669860839844</v>
       </c>
       <c r="M2" t="n">
         <v>142.7754521162054</v>
@@ -762,10 +762,10 @@
         <v>0.0001208530555588951</v>
       </c>
       <c r="K3" t="n">
-        <v>3237.819091796875</v>
+        <v>909.819091796875</v>
       </c>
       <c r="L3" t="n">
-        <v>604.118408203125</v>
+        <v>1155.881591796875</v>
       </c>
       <c r="M3" t="n">
         <v>142.8746150212031</v>
@@ -885,10 +885,10 @@
         <v>0.001025441454285217</v>
       </c>
       <c r="K4" t="n">
-        <v>1065.07421875</v>
+        <v>-1262.92578125</v>
       </c>
       <c r="L4" t="n">
-        <v>2788.794677734375</v>
+        <v>-1028.794677734375</v>
       </c>
       <c r="M4" t="n">
         <v>141.543975413795</v>
@@ -1008,10 +1008,10 @@
         <v>4.560496481182353e-05</v>
       </c>
       <c r="K5" t="n">
-        <v>1699.48388671875</v>
+        <v>-628.51611328125</v>
       </c>
       <c r="L5" t="n">
-        <v>3292.100830078125</v>
+        <v>-1532.100830078125</v>
       </c>
       <c r="M5" t="n">
         <v>141.2496959250724</v>
@@ -1131,10 +1131,10 @@
         <v>0.0002253198660929772</v>
       </c>
       <c r="K6" t="n">
-        <v>2604.37841796875</v>
+        <v>276.37841796875</v>
       </c>
       <c r="L6" t="n">
-        <v>3215.892578125</v>
+        <v>-1455.892578125</v>
       </c>
       <c r="M6" t="n">
         <v>141.3081580915755</v>
@@ -1254,10 +1254,10 @@
         <v>3.848132877426388e-05</v>
       </c>
       <c r="K7" t="n">
-        <v>4341.7421875</v>
+        <v>2013.7421875</v>
       </c>
       <c r="L7" t="n">
-        <v>1789.921875</v>
+        <v>-29.921875</v>
       </c>
       <c r="M7" t="n">
         <v>142.178840114448</v>
@@ -1377,10 +1377,10 @@
         <v>9.546265491260009e-05</v>
       </c>
       <c r="K8" t="n">
-        <v>703.9273071289062</v>
+        <v>-1624.072692871094</v>
       </c>
       <c r="L8" t="n">
-        <v>519.4584350585938</v>
+        <v>1240.541564941406</v>
       </c>
       <c r="M8" t="n">
         <v>142.9085387471616</v>
@@ -1500,10 +1500,10 @@
         <v>0.0002242493982972346</v>
       </c>
       <c r="K9" t="n">
-        <v>4400.74609375</v>
+        <v>2072.74609375</v>
       </c>
       <c r="L9" t="n">
-        <v>370.9913635253906</v>
+        <v>1389.008636474609</v>
       </c>
       <c r="M9" t="n">
         <v>143.0208411700214</v>
@@ -1623,10 +1623,10 @@
         <v>0.0002633601556291969</v>
       </c>
       <c r="K10" t="n">
-        <v>2228.3818359375</v>
+        <v>-99.6181640625</v>
       </c>
       <c r="L10" t="n">
-        <v>441.8651428222656</v>
+        <v>1318.134857177734</v>
       </c>
       <c r="M10" t="n">
         <v>142.9648759681428</v>
@@ -1746,10 +1746,10 @@
         <v>0.00024117433456986</v>
       </c>
       <c r="K11" t="n">
-        <v>2739.565673828125</v>
+        <v>411.565673828125</v>
       </c>
       <c r="L11" t="n">
-        <v>1184.418701171875</v>
+        <v>575.581298828125</v>
       </c>
       <c r="M11" t="n">
         <v>142.524494980619</v>
@@ -1869,10 +1869,10 @@
         <v>0.0001545115443973048</v>
       </c>
       <c r="K12" t="n">
-        <v>432.4064636230469</v>
+        <v>-1895.593536376953</v>
       </c>
       <c r="L12" t="n">
-        <v>1983.85205078125</v>
+        <v>-223.85205078125</v>
       </c>
       <c r="M12" t="n">
         <v>142.0223023744692</v>
@@ -1992,10 +1992,10 @@
         <v>0.0001380008170344827</v>
       </c>
       <c r="K13" t="n">
-        <v>4430.05859375</v>
+        <v>2102.05859375</v>
       </c>
       <c r="L13" t="n">
-        <v>1440.545776367188</v>
+        <v>319.4542236328125</v>
       </c>
       <c r="M13" t="n">
         <v>142.3869454008972</v>
@@ -2115,10 +2115,10 @@
         <v>8.120085062391276e-05</v>
       </c>
       <c r="K14" t="n">
-        <v>1886.18115234375</v>
+        <v>-441.81884765625</v>
       </c>
       <c r="L14" t="n">
-        <v>3066.9765625</v>
+        <v>-1306.9765625</v>
       </c>
       <c r="M14" t="n">
         <v>141.3874962747277</v>
@@ -2238,10 +2238,10 @@
         <v>0.0001566739531644443</v>
       </c>
       <c r="K15" t="n">
-        <v>913.3334350585938</v>
+        <v>-1414.666564941406</v>
       </c>
       <c r="L15" t="n">
-        <v>2154.215576171875</v>
+        <v>-394.215576171875</v>
       </c>
       <c r="M15" t="n">
         <v>141.9246550073069</v>
@@ -2361,10 +2361,10 @@
         <v>0.0002116341926834104</v>
       </c>
       <c r="K16" t="n">
-        <v>2392.8115234375</v>
+        <v>64.8115234375</v>
       </c>
       <c r="L16" t="n">
-        <v>841.6809692382812</v>
+        <v>918.3190307617188</v>
       </c>
       <c r="M16" t="n">
         <v>142.7266965755467</v>
@@ -2484,10 +2484,10 @@
         <v>0.0003618420556167934</v>
       </c>
       <c r="K17" t="n">
-        <v>1319.823608398438</v>
+        <v>-1008.176391601562</v>
       </c>
       <c r="L17" t="n">
-        <v>2766.680908203125</v>
+        <v>-1006.680908203125</v>
       </c>
       <c r="M17" t="n">
         <v>141.5605448068074</v>
@@ -2607,10 +2607,10 @@
         <v>4.039477290723064e-05</v>
       </c>
       <c r="K18" t="n">
-        <v>2516.805419921875</v>
+        <v>188.805419921875</v>
       </c>
       <c r="L18" t="n">
-        <v>503.4006652832031</v>
+        <v>1256.599334716797</v>
       </c>
       <c r="M18" t="n">
         <v>142.9299124025891</v>
@@ -2730,10 +2730,10 @@
         <v>0.0005062001456461128</v>
       </c>
       <c r="K19" t="n">
-        <v>1683.417358398438</v>
+        <v>-644.5826416015625</v>
       </c>
       <c r="L19" t="n">
-        <v>2124.171142578125</v>
+        <v>-364.171142578125</v>
       </c>
       <c r="M19" t="n">
         <v>141.9511978498535</v>
@@ -2853,10 +2853,10 @@
         <v>8.365206631862134e-05</v>
       </c>
       <c r="K20" t="n">
-        <v>1935.110107421875</v>
+        <v>-392.889892578125</v>
       </c>
       <c r="L20" t="n">
-        <v>606.6289672851562</v>
+        <v>1153.371032714844</v>
       </c>
       <c r="M20" t="n">
         <v>142.8642386761799</v>
@@ -2976,10 +2976,10 @@
         <v>5.949002359048047e-05</v>
       </c>
       <c r="K21" t="n">
-        <v>1947.955322265625</v>
+        <v>-380.044677734375</v>
       </c>
       <c r="L21" t="n">
-        <v>1063.383544921875</v>
+        <v>696.616455078125</v>
       </c>
       <c r="M21" t="n">
         <v>142.5904394233145</v>

</xml_diff>